<commit_message>
was working on propagate, that was frustrating so moving on to other things for a while.
</commit_message>
<xml_diff>
--- a/out/test_run_from_excel_at_path.xlsx
+++ b/out/test_run_from_excel_at_path.xlsx
@@ -496,21 +496,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>test loan: Interest</t>
+          <t>Checking</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>9999</v>
+        <v>100000</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>checking</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -522,7 +522,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test loan: Principal Balance</t>
+          <t>Credit: Curr Stmt Bal</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -532,32 +532,18 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>9999</v>
+        <v>20000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>principal balance</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>20000102</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>simple</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>daily</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>50</v>
-      </c>
+          <t>curr stmt bal</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -579,8 +565,10 @@
           <t>prev stmt bal</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>20000102</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +590,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Credit: Curr Stmt Bal</t>
+          <t>test loan: Principal Balance</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -612,37 +600,53 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>20000</v>
+        <v>9999</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>curr stmt bal</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+          <t>principal balance</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>simple</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>daily</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Checking</t>
+          <t>test loan: Interest</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>100000</v>
+        <v>9999</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>checking</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -713,11 +717,15 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>20000102</v>
-      </c>
-      <c r="B2" t="n">
-        <v>20000102</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -743,11 +751,15 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>20000102</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20000102</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>20000102</t>
+        </is>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -773,11 +785,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>20000104</v>
-      </c>
-      <c r="B4" t="n">
-        <v>20000104</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20000104</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>20000104</t>
+        </is>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -1246,11 +1262,15 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>20000101</v>
-      </c>
-      <c r="B2" t="n">
-        <v>20000103</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>20000101</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>20000103</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>